<commit_message>
Update to eSituation.11 and eSituation.12 suggested list.
</commit_message>
<xml_diff>
--- a/SuggestedLists/eSituation.11 and eSituation.12 - Provider Impression.xlsx
+++ b/SuggestedLists/eSituation.11 and eSituation.12 - Provider Impression.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Users\jehlers\v3.5.0 Suggested Lists\Final Lists v3.5.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\NEMSIS\NEMSIS V3\Suggested Lists_Final for v3.5.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACB1B8D2-D9EA-4D8F-AB1A-C9F8CF0233FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630F354-B8DB-4ED5-BB00-6D418EB8CAB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recommendation" sheetId="3" r:id="rId1"/>
+    <sheet name="Change Log" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Recommendation!$A$1:$E$144</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="411">
   <si>
     <t>Altered mental status</t>
   </si>
@@ -1243,13 +1244,68 @@
   </si>
   <si>
     <t>eSituation.11 and .12 - Primary and Secondary Impression Suggested List</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Illness</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, NOS</t>
+    </r>
+  </si>
+  <si>
+    <t>8/21/20 Removed. R99 already in use for Other: Obvious Death/R99/Ill-defined and unknown cause of mortality</t>
+  </si>
+  <si>
+    <t>8/21/20 "NOS" added to EMS description</t>
+  </si>
+  <si>
+    <t>Most Recent Update: 8/21/2020
+See Change Log tab for details</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Illness, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOS</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1305,6 +1361,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1326,7 +1405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1358,12 +1437,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1439,6 +1527,21 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1446,25 +1549,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1473,13 +1560,117 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1760,33 +1951,34 @@
   </sheetPr>
   <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="38.6328125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="4"/>
-    <col min="4" max="4" width="97.81640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="83" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="4"/>
+    <col min="1" max="1" width="23.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="4"/>
+    <col min="4" max="5" width="97.85546875" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>404</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="26"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="52" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>366</v>
       </c>
@@ -1799,11 +1991,11 @@
       <c r="D3" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>234</v>
       </c>
@@ -1817,7 +2009,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>257</v>
       </c>
@@ -1827,18 +2019,18 @@
       <c r="D5" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="30" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="17"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="29"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>367</v>
       </c>
@@ -1851,11 +2043,11 @@
       <c r="D7" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="30" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="11" t="s">
         <v>259</v>
@@ -1866,9 +2058,9 @@
       <c r="D8" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E8" s="29"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="9" t="s">
         <v>156</v>
@@ -1879,9 +2071,9 @@
       <c r="D9" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E9" s="27"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="11" t="s">
         <v>258</v>
@@ -1892,11 +2084,11 @@
       <c r="D10" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="30" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="25" t="s">
         <v>362</v>
@@ -1907,9 +2099,9 @@
       <c r="D11" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="E11" s="27"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="26"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="11" t="s">
         <v>260</v>
@@ -1920,9 +2112,9 @@
       <c r="D12" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="27"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E12" s="26"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="11" t="s">
         <v>294</v>
@@ -1933,16 +2125,16 @@
       <c r="D13" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E13" s="26"/>
+    </row>
+    <row r="14" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="29"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>236</v>
       </c>
@@ -1955,11 +2147,11 @@
       <c r="D15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="9" t="s">
         <v>244</v>
@@ -1970,9 +2162,9 @@
       <c r="D16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="27"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="9" t="s">
         <v>245</v>
@@ -1983,9 +2175,9 @@
       <c r="D17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="27"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>261</v>
       </c>
@@ -1995,11 +2187,11 @@
       <c r="D18" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="30" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="9" t="s">
         <v>363</v>
@@ -2010,9 +2202,9 @@
       <c r="D19" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="E19" s="32"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" s="31"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="12" t="s">
         <v>302</v>
@@ -2023,9 +2215,9 @@
       <c r="D20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="27"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E20" s="26"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="9" t="s">
         <v>14</v>
@@ -2036,9 +2228,9 @@
       <c r="D21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="27"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E21" s="26"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="9" t="s">
         <v>17</v>
@@ -2049,9 +2241,9 @@
       <c r="D22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="27"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E22" s="26"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="11" t="s">
         <v>295</v>
@@ -2062,9 +2254,9 @@
       <c r="D23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="27"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E23" s="26"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="11" t="s">
         <v>303</v>
@@ -2075,9 +2267,9 @@
       <c r="D24" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E24" s="27"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="3" t="s">
         <v>296</v>
@@ -2088,16 +2280,16 @@
       <c r="D25" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="E25" s="27"/>
-    </row>
-    <row r="26" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="26"/>
+    </row>
+    <row r="26" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="29"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E26" s="28"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>237</v>
       </c>
@@ -2110,11 +2302,11 @@
       <c r="D27" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="27" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="9" t="s">
         <v>39</v>
@@ -2125,9 +2317,9 @@
       <c r="D28" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="27"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E28" s="26"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="11" t="s">
         <v>42</v>
@@ -2138,9 +2330,9 @@
       <c r="D29" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="27"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E29" s="26"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="11" t="s">
         <v>263</v>
@@ -2151,9 +2343,9 @@
       <c r="D30" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="E30" s="27"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E30" s="26"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="11" t="s">
         <v>264</v>
@@ -2164,18 +2356,18 @@
       <c r="D31" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="30" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
       <c r="B32" s="17"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
-      <c r="E32" s="29"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E32" s="28"/>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>241</v>
       </c>
@@ -2188,11 +2380,11 @@
       <c r="D33" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="27" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="11" t="s">
         <v>307</v>
@@ -2203,11 +2395,11 @@
       <c r="D34" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="27" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="11" t="s">
         <v>403</v>
@@ -2222,7 +2414,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="11" t="s">
         <v>398</v>
@@ -2237,7 +2429,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="9" t="s">
         <v>267</v>
@@ -2248,9 +2440,9 @@
       <c r="D37" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="E37" s="27"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E37" s="26"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="11" t="s">
         <v>306</v>
@@ -2261,9 +2453,9 @@
       <c r="D38" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="27"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E38" s="26"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="11" t="s">
         <v>310</v>
@@ -2274,9 +2466,9 @@
       <c r="D39" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="E39" s="27"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E39" s="26"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="9" t="s">
         <v>269</v>
@@ -2287,9 +2479,9 @@
       <c r="D40" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E40" s="27"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E40" s="26"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="2" t="s">
         <v>200</v>
@@ -2300,16 +2492,16 @@
       <c r="D41" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E41" s="27"/>
-    </row>
-    <row r="42" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E41" s="26"/>
+    </row>
+    <row r="42" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
       <c r="B42" s="17"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="29"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E42" s="28"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>238</v>
       </c>
@@ -2322,9 +2514,9 @@
       <c r="D43" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="E43" s="27"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E43" s="26"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
       <c r="B44" s="11" t="s">
         <v>311</v>
@@ -2335,9 +2527,9 @@
       <c r="D44" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E44" s="27"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E44" s="26"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="9" t="s">
         <v>36</v>
@@ -2348,9 +2540,9 @@
       <c r="D45" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="27"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E45" s="26"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
       <c r="B46" s="11" t="s">
         <v>373</v>
@@ -2361,9 +2553,9 @@
       <c r="D46" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E46" s="27"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E46" s="26"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
       <c r="B47" s="11" t="s">
         <v>313</v>
@@ -2374,9 +2566,9 @@
       <c r="D47" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="E47" s="27"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E47" s="26"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="21"/>
       <c r="B48" s="11" t="s">
         <v>314</v>
@@ -2387,11 +2579,11 @@
       <c r="D48" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="E48" s="28" t="s">
+      <c r="E48" s="27" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="11" t="s">
         <v>315</v>
@@ -2402,16 +2594,16 @@
       <c r="D49" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="E49" s="27"/>
-    </row>
-    <row r="50" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E49" s="26"/>
+    </row>
+    <row r="50" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20"/>
       <c r="B50" s="17"/>
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
-      <c r="E50" s="29"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E50" s="28"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
         <v>235</v>
       </c>
@@ -2424,9 +2616,9 @@
       <c r="D51" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="27"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E51" s="26"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>316</v>
       </c>
@@ -2436,11 +2628,11 @@
       <c r="D52" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="E52" s="27"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B53" s="9" t="s">
-        <v>235</v>
+      <c r="E52" s="26"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="42" t="s">
+        <v>410</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>179</v>
@@ -2448,9 +2640,11 @@
       <c r="D53" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="E53" s="27"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E53" s="39" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="11" t="s">
         <v>317</v>
@@ -2461,21 +2655,23 @@
       <c r="D54" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E54" s="27"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B55" s="9" t="s">
+      <c r="E54" s="26"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="40" t="s">
         <v>271</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="E55" s="27"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E55" s="39" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
       <c r="B56" s="11" t="s">
         <v>74</v>
@@ -2486,16 +2682,16 @@
       <c r="D56" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E56" s="27"/>
-    </row>
-    <row r="57" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E56" s="26"/>
+    </row>
+    <row r="57" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20"/>
       <c r="B57" s="17"/>
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
-      <c r="E57" s="29"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E57" s="28"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>77</v>
       </c>
@@ -2508,9 +2704,9 @@
       <c r="D58" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E58" s="27"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E58" s="26"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="9" t="s">
         <v>332</v>
       </c>
@@ -2520,9 +2716,9 @@
       <c r="D59" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E59" s="27"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E59" s="26"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" s="9" t="s">
         <v>365</v>
       </c>
@@ -2532,9 +2728,9 @@
       <c r="D60" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E60" s="27"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E60" s="26"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="9" t="s">
         <v>364</v>
       </c>
@@ -2544,11 +2740,11 @@
       <c r="D61" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E61" s="32" t="s">
+      <c r="E61" s="31" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" s="9" t="s">
         <v>331</v>
       </c>
@@ -2558,11 +2754,11 @@
       <c r="D62" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="E62" s="28" t="s">
+      <c r="E62" s="27" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" s="9" t="s">
         <v>274</v>
       </c>
@@ -2572,9 +2768,9 @@
       <c r="D63" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E63" s="27"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E63" s="26"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" s="9" t="s">
         <v>327</v>
       </c>
@@ -2584,9 +2780,9 @@
       <c r="D64" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E64" s="27"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E64" s="26"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" s="9" t="s">
         <v>323</v>
       </c>
@@ -2596,9 +2792,9 @@
       <c r="D65" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E65" s="27"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E65" s="26"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" s="9" t="s">
         <v>273</v>
       </c>
@@ -2608,11 +2804,11 @@
       <c r="D66" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E66" s="28" t="s">
+      <c r="E66" s="27" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>318</v>
       </c>
@@ -2622,9 +2818,9 @@
       <c r="D67" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="E67" s="27"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E67" s="26"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" s="9" t="s">
         <v>324</v>
       </c>
@@ -2634,9 +2830,9 @@
       <c r="D68" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E68" s="27"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E68" s="26"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>109</v>
       </c>
@@ -2646,11 +2842,11 @@
       <c r="D69" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E69" s="31" t="s">
+      <c r="E69" s="30" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
         <v>329</v>
       </c>
@@ -2661,7 +2857,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
         <v>328</v>
       </c>
@@ -2672,7 +2868,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" s="9" t="s">
         <v>111</v>
       </c>
@@ -2683,7 +2879,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="s">
         <v>320</v>
       </c>
@@ -2694,7 +2890,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" s="9" t="s">
         <v>322</v>
       </c>
@@ -2705,7 +2901,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
         <v>275</v>
       </c>
@@ -2716,7 +2912,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
         <v>325</v>
       </c>
@@ -2727,7 +2923,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
         <v>321</v>
       </c>
@@ -2738,7 +2934,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="9" t="s">
         <v>276</v>
       </c>
@@ -2749,13 +2945,13 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="20"/>
       <c r="B79" s="17"/>
       <c r="C79" s="18"/>
       <c r="D79" s="18"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>239</v>
       </c>
@@ -2769,7 +2965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" s="9" t="s">
         <v>252</v>
       </c>
@@ -2780,7 +2976,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" s="9" t="s">
         <v>358</v>
       </c>
@@ -2791,7 +2987,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" s="9" t="s">
         <v>251</v>
       </c>
@@ -2802,13 +2998,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="20"/>
       <c r="B84" s="17"/>
       <c r="C84" s="18"/>
       <c r="D84" s="18"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>61</v>
       </c>
@@ -2822,7 +3018,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
       <c r="B86" s="9" t="s">
         <v>341</v>
@@ -2834,7 +3030,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
       <c r="B87" s="12" t="s">
         <v>333</v>
@@ -2846,7 +3042,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="22"/>
       <c r="B88" s="9" t="s">
         <v>71</v>
@@ -2858,13 +3054,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="20"/>
       <c r="B89" s="17"/>
       <c r="C89" s="18"/>
       <c r="D89" s="18"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>243</v>
       </c>
@@ -2878,7 +3074,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" s="9" t="s">
         <v>64</v>
       </c>
@@ -2889,13 +3085,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="20"/>
       <c r="B92" s="17"/>
       <c r="C92" s="18"/>
       <c r="D92" s="18"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>240</v>
       </c>
@@ -2909,7 +3105,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="15" t="s">
         <v>253</v>
       </c>
@@ -2920,7 +3116,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="21"/>
       <c r="B95" s="11" t="s">
         <v>335</v>
@@ -2932,7 +3128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="21"/>
       <c r="B96" s="11" t="s">
         <v>336</v>
@@ -2944,7 +3140,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="21"/>
       <c r="B97" s="11" t="s">
         <v>342</v>
@@ -2956,7 +3152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="21"/>
       <c r="B98" s="9" t="s">
         <v>26</v>
@@ -2968,7 +3164,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="21"/>
       <c r="B99" s="11" t="s">
         <v>29</v>
@@ -2980,13 +3176,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="20"/>
       <c r="B100" s="17"/>
       <c r="C100" s="18"/>
       <c r="D100" s="18"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
         <v>114</v>
       </c>
@@ -3000,7 +3196,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="21"/>
       <c r="B102" s="11" t="s">
         <v>343</v>
@@ -3012,7 +3208,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="21"/>
       <c r="B103" s="11" t="s">
         <v>347</v>
@@ -3024,7 +3220,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="21"/>
       <c r="B104" s="11" t="s">
         <v>348</v>
@@ -3036,7 +3232,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="21"/>
       <c r="B105" s="9" t="s">
         <v>278</v>
@@ -3048,7 +3244,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="21"/>
       <c r="B106" s="9" t="s">
         <v>346</v>
@@ -3060,7 +3256,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="21"/>
       <c r="B107" s="11" t="s">
         <v>344</v>
@@ -3072,7 +3268,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="21"/>
       <c r="B108" s="11" t="s">
         <v>345</v>
@@ -3084,13 +3280,13 @@
         <v>222</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="20"/>
       <c r="B109" s="17"/>
       <c r="C109" s="18"/>
       <c r="D109" s="18"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="22" t="s">
         <v>233</v>
       </c>
@@ -3107,7 +3303,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="22"/>
       <c r="B111" s="12" t="s">
         <v>360</v>
@@ -3119,7 +3315,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="22"/>
       <c r="B112" s="12" t="s">
         <v>56</v>
@@ -3131,7 +3327,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="22"/>
       <c r="B113" s="12" t="s">
         <v>371</v>
@@ -3143,7 +3339,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="22"/>
       <c r="B114" s="12" t="s">
         <v>359</v>
@@ -3155,7 +3351,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="22"/>
       <c r="B115" s="12" t="s">
         <v>374</v>
@@ -3167,13 +3363,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="20"/>
       <c r="B116" s="17"/>
       <c r="C116" s="18"/>
       <c r="D116" s="18"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>119</v>
       </c>
@@ -3187,7 +3383,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B118" s="9" t="s">
         <v>128</v>
       </c>
@@ -3198,7 +3394,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B119" s="9" t="s">
         <v>285</v>
       </c>
@@ -3208,11 +3404,11 @@
       <c r="D119" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="E119" s="36" t="s">
+      <c r="E119" s="35" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="22"/>
       <c r="B120" s="9" t="s">
         <v>282</v>
@@ -3223,9 +3419,9 @@
       <c r="D120" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="E120" s="33"/>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E120" s="32"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="22"/>
       <c r="B121" s="9" t="s">
         <v>338</v>
@@ -3236,9 +3432,9 @@
       <c r="D121" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E121" s="33"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E121" s="32"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="22"/>
       <c r="B122" s="9" t="s">
         <v>339</v>
@@ -3249,9 +3445,9 @@
       <c r="D122" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E122" s="35"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E122" s="34"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B123" s="9" t="s">
         <v>340</v>
       </c>
@@ -3261,9 +3457,9 @@
       <c r="D123" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="E123" s="37"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E123" s="36"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="22"/>
       <c r="B124" s="16" t="s">
         <v>281</v>
@@ -3274,11 +3470,11 @@
       <c r="D124" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E124" s="34" t="s">
+      <c r="E124" s="33" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B125" s="9" t="s">
         <v>288</v>
       </c>
@@ -3288,16 +3484,16 @@
       <c r="D125" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="E125" s="33"/>
-    </row>
-    <row r="126" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E125" s="32"/>
+    </row>
+    <row r="126" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="20"/>
       <c r="B126" s="17"/>
       <c r="C126" s="18"/>
       <c r="D126" s="18"/>
-      <c r="E126" s="35"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E126" s="34"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="22" t="s">
         <v>242</v>
       </c>
@@ -3310,9 +3506,9 @@
       <c r="D127" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="E127" s="33"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E127" s="32"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="22"/>
       <c r="B128" s="12" t="s">
         <v>292</v>
@@ -3323,9 +3519,9 @@
       <c r="D128" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="E128" s="33"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E128" s="32"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="22"/>
       <c r="B129" s="9" t="s">
         <v>372</v>
@@ -3336,16 +3532,16 @@
       <c r="D129" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E129" s="33"/>
-    </row>
-    <row r="130" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E129" s="32"/>
+    </row>
+    <row r="130" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="20"/>
       <c r="B130" s="17"/>
       <c r="C130" s="18"/>
       <c r="D130" s="18"/>
-      <c r="E130" s="35"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E130" s="34"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="21" t="s">
         <v>134</v>
       </c>
@@ -3358,11 +3554,11 @@
       <c r="D131" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="E131" s="34" t="s">
+      <c r="E131" s="33" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="21"/>
       <c r="B132" s="11" t="s">
         <v>354</v>
@@ -3373,9 +3569,9 @@
       <c r="D132" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E132" s="33"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E132" s="32"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="21"/>
       <c r="B133" s="11" t="s">
         <v>137</v>
@@ -3386,9 +3582,9 @@
       <c r="D133" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E133" s="33"/>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E133" s="32"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="21"/>
       <c r="B134" s="11" t="s">
         <v>349</v>
@@ -3399,11 +3595,11 @@
       <c r="D134" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E134" s="34" t="s">
+      <c r="E134" s="33" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B135" s="9" t="s">
         <v>291</v>
       </c>
@@ -3413,9 +3609,9 @@
       <c r="D135" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E135" s="33"/>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E135" s="32"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="21"/>
       <c r="B136" s="11" t="s">
         <v>293</v>
@@ -3426,22 +3622,22 @@
       <c r="D136" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="E136" s="33"/>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E136" s="32"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="21"/>
       <c r="B137" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="C137" s="38" t="s">
+      <c r="C137" s="37" t="s">
         <v>149</v>
       </c>
       <c r="D137" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E137" s="33"/>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E137" s="32"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="22"/>
       <c r="B138" s="9" t="s">
         <v>206</v>
@@ -3452,9 +3648,9 @@
       <c r="D138" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E138" s="33"/>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E138" s="32"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="21"/>
       <c r="B139" s="11" t="s">
         <v>146</v>
@@ -3465,9 +3661,9 @@
       <c r="D139" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="E139" s="33"/>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E139" s="32"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="21"/>
       <c r="B140" s="9" t="s">
         <v>290</v>
@@ -3478,9 +3674,9 @@
       <c r="D140" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E140" s="33"/>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E140" s="32"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="21"/>
       <c r="B141" s="11" t="s">
         <v>353</v>
@@ -3492,7 +3688,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="21"/>
       <c r="B142" s="11" t="s">
         <v>355</v>
@@ -3504,7 +3700,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B143" s="9" t="s">
         <v>176</v>
       </c>
@@ -3525,4 +3721,94 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3193AA49-E1C3-4819-A8A1-553357C9B204}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="112.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="43" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>366</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49">
+        <v>44064</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="49">
+        <v>44064</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>407</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates Suggested Lists for eMedications.03, eProcedures.03 and eSituation.11
</commit_message>
<xml_diff>
--- a/SuggestedLists/eSituation.11 and eSituation.12 - Provider Impression.xlsx
+++ b/SuggestedLists/eSituation.11 and eSituation.12 - Provider Impression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\NEMSIS\NEMSIS V3\Suggested Lists_Final for v3.5.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630F354-B8DB-4ED5-BB00-6D418EB8CAB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D070A4-3AC0-4FD4-BCE2-371C5322F67C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recommendation" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Recommendation!$A$1:$E$144</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="414">
   <si>
     <t>Altered mental status</t>
   </si>
@@ -1232,9 +1232,6 @@
   </si>
   <si>
     <t>Intentional self-harm by other specified means</t>
-  </si>
-  <si>
-    <t>8/29 added to address clinicians ability to clearly describe impression</t>
   </si>
   <si>
     <t>8/29 removed "and suicidal" from EMS Description, already covered in R45.851</t>
@@ -1276,10 +1273,6 @@
     <t>8/21/20 "NOS" added to EMS description</t>
   </si>
   <si>
-    <t>Most Recent Update: 8/21/2020
-See Change Log tab for details</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1300,12 +1293,40 @@
       <t>NOS</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8/29 added to address clinicians ability to clearly describe impression; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11/20/2020 Removed from list, forbidden by the NEMSIS XSD's regex rule.</t>
+    </r>
+  </si>
+  <si>
+    <t>Most Recent Update: 11/20/2020
+See Change Log tab for details</t>
+  </si>
+  <si>
+    <t>11/20/2020 Removed from list, forbidden by the NEMSIS XSD's regex rule.</t>
+  </si>
+  <si>
+    <t>8/21/20 "NOS" added to EMS description.</t>
+  </si>
+  <si>
+    <t>8/21/20 Removed. R99 already in use for Other: Obvious Death/R99/Ill-defined and unknown cause of mortality.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1384,6 +1405,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1451,7 +1479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1558,9 +1586,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1604,42 +1629,36 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1951,8 +1970,8 @@
   </sheetPr>
   <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,14 +1984,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>404</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="52" t="s">
-        <v>409</v>
+      <c r="A1" s="56" t="s">
+        <v>403</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="51" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2402,7 +2421,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>220</v>
@@ -2411,22 +2430,22 @@
         <v>219</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="11" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="53" t="s">
         <v>398</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="52" t="s">
         <v>399</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="52" t="s">
         <v>400</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2631,8 +2650,8 @@
       <c r="E52" s="26"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="42" t="s">
-        <v>410</v>
+      <c r="B53" s="41" t="s">
+        <v>408</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>179</v>
@@ -2640,8 +2659,8 @@
       <c r="D53" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="E53" s="39" t="s">
-        <v>408</v>
+      <c r="E53" s="38" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,17 +2677,17 @@
       <c r="E54" s="26"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="C55" s="53" t="s">
+      <c r="C55" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="D55" s="41" t="s">
+      <c r="D55" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E55" s="39" t="s">
-        <v>407</v>
+      <c r="E55" s="38" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3724,90 +3743,113 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3193AA49-E1C3-4819-A8A1-553357C9B204}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="112.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="58" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="58" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="58"/>
+    <col min="5" max="5" width="40.7109375" style="58" customWidth="1"/>
+    <col min="6" max="6" width="112.28515625" style="58" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="43" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:6" s="42" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
+        <v>404</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>366</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>356</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>357</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="48">
+        <v>44064</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="44" t="s">
         <v>405</v>
       </c>
-      <c r="B1" s="44" t="s">
-        <v>366</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>361</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>356</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>357</v>
-      </c>
-      <c r="F1" s="44" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49">
+      <c r="D2" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="48">
         <v>44064</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="45" t="s">
-        <v>406</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E2" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" s="51" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49">
-        <v>44064</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="46" t="s">
         <v>271</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>407</v>
+      <c r="F3" s="50" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="57">
+        <v>44155</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>398</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>399</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>400</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>